<commit_message>
Finished testing buyout functionality
</commit_message>
<xml_diff>
--- a/SaucedemoTestData.xlsx
+++ b/SaucedemoTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mladj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\IdeaProjects\ITBootcampProjects\ItbProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495F44FE-258B-41F7-8E24-72CCCADF111A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E19DE65-7869-4546-A443-01C4B907AFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,10 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +427,7 @@
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -449,7 +450,7 @@
       <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -472,7 +473,7 @@
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>123456</v>
       </c>
     </row>

</xml_diff>